<commit_message>
Added metadata for 01 July 2021 height / level changes
</commit_message>
<xml_diff>
--- a/metadata/wind_profile_metadata.xlsx
+++ b/metadata/wind_profile_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB287D10-6C67-2C44-A629-E7A06A7CB3EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B0B760-1699-3849-8E16-A0E4AF56E3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39100" yWindow="-3140" windowWidth="26380" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39100" yWindow="-10580" windowWidth="26380" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global-attributes" sheetId="1" r:id="rId1"/>
@@ -214,13 +214,7 @@
     <t>Data collection start: 2019-06-01T00:00:00</t>
   </si>
   <si>
-    <t>Platform height (h0) is the top of the Met tower. Instrument height: M1=h0-12.3m, V1=h0-9.8m,M2=h0-4.5m, V2=h0-1m ,.</t>
-  </si>
-  <si>
     <t>N/a</t>
-  </si>
-  <si>
-    <t>Point measurements of temperature/ humidity from HMP155 sensors at four levels on the Summit Station met tower.</t>
   </si>
   <si>
     <t>https://github.com/heatherguy/ace-ceda-master</t>
@@ -268,6 +262,12 @@
   </si>
   <si>
     <t>timeSeries</t>
+  </si>
+  <si>
+    <t>Point measurements of wind speed / direction from 2D and 3D sonic anemometers on four levels on the Summit Station met tower.</t>
+  </si>
+  <si>
+    <t>Platform height (h0) is the top of the Met tower. Instrument height: M1=h0-12.3m, V1=h0-9.8m,V2=h0-4.5m, M2=h0-1m ,.</t>
   </si>
 </sst>
 </file>
@@ -718,7 +718,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -741,7 +741,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -773,7 +773,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -781,7 +781,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -789,7 +789,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -829,7 +829,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -853,7 +853,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -861,7 +861,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -947,7 +947,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -979,7 +979,7 @@
         <v>36</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -987,7 +987,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1007,7 +1007,7 @@
         <v>40</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -1050,7 +1050,7 @@
         <v>44</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>